<commit_message>
adding new drill to older file
</commit_message>
<xml_diff>
--- a/SoccerDrillsList_old.xlsx
+++ b/SoccerDrillsList_old.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergejs_Sushinskis\Documents\soccer\06092025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergejs_Sushinskis\Documents\soccer\soccer_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F46D166-70FA-4816-9E23-72B6104711DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70D90D-B184-4D73-89C2-146600E5036E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="drills list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'drills list'!$A$1:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'drills list'!$A$1:$I$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Nr</t>
   </si>
@@ -325,6 +325,37 @@
   </si>
   <si>
     <t>https://youtube.com/shorts/fi2AqhSWytk?feature=share</t>
+  </si>
+  <si>
+    <t>Combination Passing &amp; Shooting Drill</t>
+  </si>
+  <si>
+    <t>Players line up at the starting cone. Player A (1) passes forward to Player B (2) at the first cone. Player B immediately plays the ball out wide to Player C (3) positioned on the side cone. Player C takes a positive touch, drives towards goal, and shoots. After each action, players rotate by following their pass: passer moves to the next cone, shooter returns to join the back of the starting line. The next round repeats the same pattern on the opposite side, alternating right and left.</t>
+  </si>
+  <si>
+    <t>- Quality of passing (accuracy, pace, and timing).
+- Movement off the ball (quick support, awareness of rotation).
+- First touch into space to set up the shot.
+- Shooting technique: composure, striking with accuracy and power.
+- Encourage players to scan and adjust body position before receiving.</t>
+  </si>
+  <si>
+    <t>https://youtube.com/shorts/Seib5Ps9gNE</t>
+  </si>
+  <si>
+    <t>Half pitch. One cone as the starting point, one cone 6–8m ahead, two side cones staggered wider towards the edge of the box, and a goal with GK. Mannequins/poles can be placed centrally to simulate defenders.</t>
+  </si>
+  <si>
+    <t>6–12 players + goalkeeper.</t>
+  </si>
+  <si>
+    <t>- Restrict to one-touch passing between cones.
+- Shooter must finish with weaker foot.
+- Add passive defender(s) to pressure shooter.
+- Introduce competition between sides (first to 5 goals).</t>
+  </si>
+  <si>
+    <t>Improve combination play, forward passing, movement off the ball, and finishing under minimal pressure</t>
   </si>
 </sst>
 </file>
@@ -474,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -515,6 +546,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,8 +597,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Drills_list" displayName="Drills_list" ref="A1:I3">
-  <autoFilter ref="A1:I3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Drills_list" displayName="Drills_list" ref="A1:I5">
+  <autoFilter ref="A1:I5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nr"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
@@ -783,11 +815,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -916,20 +948,50 @@
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
     </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Warm-Up,Dribbling / Ball Control,Passing &amp; Receiving,Shooting / Finishing,1v1 / Defending,Small-Sided Games,Coordination &amp; Agility,Cool Down / Fun Game,Attacking"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="D2:D5" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{82182842-0E7B-48DD-B438-8448282F1EAB}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{57D41271-A300-479A-A9D9-37C3F72A690D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>